<commit_message>
fixed #115 TournRPG-115 全体攻撃の実装
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -443,7 +443,7 @@
     <t>ATK_PHY</t>
   </si>
   <si>
-    <t>敵単</t>
+    <t>ENEMY_ONE</t>
   </si>
   <si>
     <t>AT_PHY</t>
@@ -476,7 +476,7 @@
     <t>ATK_BST</t>
   </si>
   <si>
-    <t>敵全</t>
+    <t>ENEMY_ALL</t>
   </si>
   <si>
     <t>AT_POISON</t>
@@ -497,7 +497,7 @@
     <t>RECOVER</t>
   </si>
   <si>
-    <t>味単</t>
+    <t>FRIEND_ONE</t>
   </si>
   <si>
     <t>HPを小回復</t>
@@ -512,7 +512,7 @@
     <t>BUFF</t>
   </si>
   <si>
-    <t>味全</t>
+    <t>FRIEND_ALL</t>
   </si>
   <si>
     <t>攻撃力アップ</t>
@@ -1975,7 +1975,7 @@
     <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="2.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="2.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.875" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.75" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
fixed #143 TournRPG-143 初期スキルを変更する
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -437,22 +437,31 @@
     <t>SKILL001</t>
   </si>
   <si>
+    <t>大斬り</t>
+  </si>
+  <si>
+    <t>ATK_PHY</t>
+  </si>
+  <si>
+    <t>ENEMY_ONE</t>
+  </si>
+  <si>
+    <t>AT_PHY</t>
+  </si>
+  <si>
+    <t>敵1体に強力な攻撃をする</t>
+  </si>
+  <si>
+    <t>SKILL002</t>
+  </si>
+  <si>
     <t>二段攻撃</t>
   </si>
   <si>
-    <t>ATK_PHY</t>
-  </si>
-  <si>
-    <t>ENEMY_ONE</t>
-  </si>
-  <si>
-    <t>AT_PHY</t>
-  </si>
-  <si>
-    <t>2回攻撃</t>
-  </si>
-  <si>
-    <t>SKILL002</t>
+    <t>敵1体に2回攻撃をする</t>
+  </si>
+  <si>
+    <t>SKILL003</t>
   </si>
   <si>
     <t>魔弾</t>
@@ -467,7 +476,7 @@
     <t>火炎属性の小ダメージ</t>
   </si>
   <si>
-    <t>SKILL003</t>
+    <t>SKILL004</t>
   </si>
   <si>
     <t>毒の粉</t>
@@ -488,7 +497,7 @@
     <t>敵全体に一定確率で毒</t>
   </si>
   <si>
-    <t>SKILL004</t>
+    <t>SKILL005</t>
   </si>
   <si>
     <t>HP回復</t>
@@ -503,7 +512,7 @@
     <t>HPを小回復</t>
   </si>
   <si>
-    <t>SKILL005</t>
+    <t>SKILL006</t>
   </si>
   <si>
     <t>攻撃アップ</t>
@@ -1962,7 +1971,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
@@ -2128,7 +2137,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" t="s" s="5">
@@ -2138,13 +2147,13 @@
         <v>26</v>
       </c>
       <c r="H3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="6">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="K3" s="6">
         <v>130</v>
@@ -2169,26 +2178,26 @@
         <v>29</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6">
-        <v>3</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D4" s="5">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" t="s" s="5">
         <v>25</v>
       </c>
       <c r="G4" t="s" s="5">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="6">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="K4" s="6">
         <v>130</v>
@@ -2202,28 +2211,28 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" t="s" s="5">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s" s="5">
         <v>33</v>
-      </c>
-      <c r="B5" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s" s="5">
-        <v>35</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6">
         <v>3</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -2231,96 +2240,140 @@
       <c r="I5" s="6">
         <v>1</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="M5" s="6">
-        <v>60</v>
-      </c>
-      <c r="N5" s="6">
-        <v>25</v>
-      </c>
+      <c r="J5" s="6">
+        <v>110</v>
+      </c>
+      <c r="K5" s="6">
+        <v>130</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
       <c r="T5" t="s" s="5">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="6">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s" s="5">
         <v>40</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" t="s" s="5">
+        <v>41</v>
+      </c>
+      <c r="M6" s="6">
+        <v>60</v>
+      </c>
+      <c r="N6" s="6">
+        <v>25</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
       <c r="T6" t="s" s="5">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s" s="5">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s" s="5">
         <v>45</v>
-      </c>
-      <c r="B7" t="s" s="5">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s" s="5">
-        <v>47</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s" s="5">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="6">
-        <v>1</v>
-      </c>
+      <c r="O7" s="6">
+        <v>40</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" t="s" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s" s="5">
         <v>49</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>50</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s" s="5">
+        <v>51</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="6">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" t="s" s="5">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2381,19 +2434,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K1" t="s" s="2">
         <v>6</v>
@@ -2454,13 +2507,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
@@ -2477,18 +2530,18 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" t="s" s="5">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -2503,18 +2556,18 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" t="s" s="5">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
@@ -2529,18 +2582,18 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" t="s" s="5">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s" s="5">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>68</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>65</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -2555,7 +2608,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" t="s" s="5">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #167 TournRPG-167 眠り状態の実装
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -525,6 +525,21 @@
   </si>
   <si>
     <t>攻撃力アップ</t>
+  </si>
+  <si>
+    <t>SKILL007</t>
+  </si>
+  <si>
+    <t>子守歌</t>
+  </si>
+  <si>
+    <t>AT_SLEEP</t>
+  </si>
+  <si>
+    <t>sleep</t>
+  </si>
+  <si>
+    <t>敵全体を一定確率で眠らせる</t>
   </si>
   <si>
     <t>rec_hp</t>
@@ -1971,7 +1986,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
@@ -2374,6 +2389,50 @@
       <c r="S8" s="7"/>
       <c r="T8" t="s" s="5">
         <v>52</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s" s="5">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s" s="5">
+        <v>55</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
+      <c r="L9" t="s" s="5">
+        <v>56</v>
+      </c>
+      <c r="M9" s="6">
+        <v>60</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" t="s" s="5">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2434,19 +2493,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s" s="2">
         <v>6</v>
@@ -2507,13 +2566,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
@@ -2530,18 +2589,18 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" t="s" s="5">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -2556,18 +2615,18 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" t="s" s="5">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
@@ -2582,18 +2641,18 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" t="s" s="5">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -2608,7 +2667,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" t="s" s="5">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #168 TournRPG-168 暗闇状態の実装
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>id</t>
   </si>
@@ -540,6 +540,21 @@
   </si>
   <si>
     <t>敵全体を一定確率で眠らせる</t>
+  </si>
+  <si>
+    <t>SKILL008</t>
+  </si>
+  <si>
+    <t>目つぶし</t>
+  </si>
+  <si>
+    <t>AT_BLIND</t>
+  </si>
+  <si>
+    <t>blind</t>
+  </si>
+  <si>
+    <t>相手を暗闇状態にする</t>
   </si>
   <si>
     <t>rec_hp</t>
@@ -1986,7 +2001,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
@@ -2433,6 +2448,50 @@
       <c r="S9" s="7"/>
       <c r="T9" t="s" s="5">
         <v>57</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s" s="5">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s" s="5">
+        <v>60</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" t="s" s="5">
+        <v>61</v>
+      </c>
+      <c r="M10" s="6">
+        <v>60</v>
+      </c>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" t="s" s="5">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2493,19 +2552,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s" s="2">
         <v>6</v>
@@ -2566,13 +2625,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
@@ -2589,18 +2648,18 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" t="s" s="5">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -2615,18 +2674,18 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" t="s" s="5">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
@@ -2641,18 +2700,18 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" t="s" s="5">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -2667,7 +2726,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" t="s" s="5">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #171 TournRPG-171 封印状態の実装
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
   <si>
     <t>id</t>
   </si>
@@ -555,6 +555,21 @@
   </si>
   <si>
     <t>相手を暗闇状態にする</t>
+  </si>
+  <si>
+    <t>SKILL009</t>
+  </si>
+  <si>
+    <t>サイレント</t>
+  </si>
+  <si>
+    <t>AT_CLOSE</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>相手のスキルを封印する</t>
   </si>
   <si>
     <t>rec_hp</t>
@@ -2001,7 +2016,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
@@ -2492,6 +2507,50 @@
       <c r="S10" s="7"/>
       <c r="T10" t="s" s="5">
         <v>62</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s" s="5">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s" s="5">
+        <v>65</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" t="s" s="5">
+        <v>66</v>
+      </c>
+      <c r="M11" s="6">
+        <v>60</v>
+      </c>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" t="s" s="5">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2552,19 +2611,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K1" t="s" s="2">
         <v>6</v>
@@ -2625,13 +2684,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
@@ -2648,18 +2707,18 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" t="s" s="5">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -2674,18 +2733,18 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" t="s" s="5">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
@@ -2700,18 +2759,18 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" t="s" s="5">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -2726,7 +2785,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" t="s" s="5">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #183 TournRPG-183 バフスキルの実装
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -437,7 +437,7 @@
     <t>SKILL001</t>
   </si>
   <si>
-    <t>大斬り</t>
+    <t>かみつき</t>
   </si>
   <si>
     <t>ATK_PHY</t>
@@ -500,7 +500,7 @@
     <t>SKILL005</t>
   </si>
   <si>
-    <t>HP回復</t>
+    <t>ヒーリング</t>
   </si>
   <si>
     <t>RECOVER</t>
@@ -515,7 +515,7 @@
     <t>SKILL006</t>
   </si>
   <si>
-    <t>攻撃アップ</t>
+    <t>パワーアップ</t>
   </si>
   <si>
     <t>BUFF</t>
@@ -524,7 +524,7 @@
     <t>FRIEND_ALL</t>
   </si>
   <si>
-    <t>攻撃力アップ</t>
+    <t>攻撃力をアップする</t>
   </si>
   <si>
     <t>SKILL007</t>

</xml_diff>

<commit_message>
fixed #184 TournRPG-184 デバフスキルの実装
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -515,7 +515,7 @@
     <t>SKILL006</t>
   </si>
   <si>
-    <t>パワーアップ</t>
+    <t>力こぶし</t>
   </si>
   <si>
     <t>BUFF</t>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>相手のスキルを封印する</t>
+  </si>
+  <si>
+    <t>SKILL010</t>
+  </si>
+  <si>
+    <t>パワーダウン</t>
+  </si>
+  <si>
+    <t>敵全体の攻撃力を下げる</t>
   </si>
   <si>
     <t>rec_hp</t>
@@ -2016,7 +2025,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
@@ -2025,7 +2034,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="2.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="2.875" style="1" customWidth="1"/>
@@ -2551,6 +2560,42 @@
       <c r="S11" s="7"/>
       <c r="T11" t="s" s="5">
         <v>67</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s" s="5">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>50</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" t="s" s="5">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2611,19 +2656,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K1" t="s" s="2">
         <v>6</v>
@@ -2684,13 +2729,13 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
@@ -2707,18 +2752,18 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" t="s" s="5">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D4" s="5">
         <v>10</v>
@@ -2733,18 +2778,18 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" t="s" s="5">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
@@ -2759,18 +2804,18 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" t="s" s="5">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s" s="5">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>86</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>83</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
@@ -2785,7 +2830,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" t="s" s="5">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #234 TournRPG-234 購入・売却金額の表示
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
   <si>
     <t>id</t>
   </si>
@@ -423,6 +423,12 @@
   </si>
   <si>
     <t>buff_spd</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>sell</t>
   </si>
   <si>
     <t>detail</t>
@@ -648,11 +654,11 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -683,11 +689,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -739,29 +740,32 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -852,53 +856,8 @@
         <a:cs typeface="ヒラギノ角ゴ ProN W3"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Blank">
       <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="129999"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -967,27 +926,6 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="104999"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
@@ -1017,83 +955,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1164,12 +1027,13 @@
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1458,6 +1322,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -1739,12 +1604,13 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -2025,35 +1891,37 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
+      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="2.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="4.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.25" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.25" style="1" customWidth="1"/>
-    <col min="15" max="15" width="2.875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.25" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6.375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6.625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="31.2812" style="1" customWidth="1"/>
-    <col min="21" max="256" width="9" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.17188" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.35156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.35156" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.35156" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.35156" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.35156" style="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85156" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.35156" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85156" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.75" style="1" customWidth="1"/>
+    <col min="22" max="22" width="41.6875" style="1" customWidth="1"/>
+    <col min="23" max="256" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -2117,489 +1985,571 @@
       <c r="T1" t="s" s="2">
         <v>19</v>
       </c>
+      <c r="U1" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="R2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T2" t="s" s="4">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="U2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="V2" t="s" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5">
+        <v>26</v>
+      </c>
+      <c r="D3" s="6">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
       <c r="F3" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="H3" s="6">
+        <v>28</v>
+      </c>
+      <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="7">
         <v>1</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="7">
         <v>50</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="7">
         <v>130</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" t="s" s="5">
-        <v>27</v>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="7">
+        <v>100</v>
+      </c>
+      <c r="U3" s="7">
+        <f>T3*0.5</f>
+        <v>50</v>
+      </c>
+      <c r="V3" t="s" s="5">
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s" s="5">
         <v>28</v>
       </c>
-      <c r="B4" t="s" s="5">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" t="s" s="5">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="7">
         <v>2</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="7">
         <v>35</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="7">
         <v>130</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" t="s" s="5">
-        <v>30</v>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="7">
+        <v>150</v>
+      </c>
+      <c r="U4" s="7">
+        <f>T4*0.5</f>
+        <v>75</v>
+      </c>
+      <c r="V4" t="s" s="5">
+        <v>32</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>33</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6">
+        <v>35</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7">
         <v>3</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="H5" s="6">
+        <v>36</v>
+      </c>
+      <c r="H5" s="7">
         <v>1</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="7">
         <v>1</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="7">
         <v>110</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="7">
         <v>130</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" t="s" s="5">
-        <v>35</v>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="7">
+        <v>200</v>
+      </c>
+      <c r="U5" s="7">
+        <f>T5*0.5</f>
+        <v>100</v>
+      </c>
+      <c r="V5" t="s" s="5">
+        <v>37</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7">
         <v>3</v>
       </c>
       <c r="F6" t="s" s="5">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s" s="5">
-        <v>40</v>
-      </c>
-      <c r="H6" s="6">
+        <v>42</v>
+      </c>
+      <c r="H6" s="7">
         <v>1</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="7">
         <v>1</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
       <c r="L6" t="s" s="5">
-        <v>41</v>
-      </c>
-      <c r="M6" s="6">
+        <v>43</v>
+      </c>
+      <c r="M6" s="7">
         <v>60</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="7">
         <v>25</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" t="s" s="5">
-        <v>42</v>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7">
+        <v>250</v>
+      </c>
+      <c r="U6" s="7">
+        <f>T6*0.5</f>
+        <v>125</v>
+      </c>
+      <c r="V6" t="s" s="5">
+        <v>44</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>45</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6">
+        <v>47</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7">
         <v>5</v>
       </c>
       <c r="F7" t="s" s="5">
-        <v>46</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="6">
+        <v>48</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="7">
         <v>40</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" t="s" s="5">
-        <v>47</v>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="7">
+        <v>300</v>
+      </c>
+      <c r="U7" s="7">
+        <f>T7*0.5</f>
+        <v>150</v>
+      </c>
+      <c r="V7" t="s" s="5">
+        <v>49</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>50</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6">
+        <v>52</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7">
         <v>7</v>
       </c>
       <c r="F8" t="s" s="5">
-        <v>51</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="6">
+        <v>53</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="7">
         <v>1</v>
       </c>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" t="s" s="5">
-        <v>52</v>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="7">
+        <v>350</v>
+      </c>
+      <c r="U8" s="7">
+        <f>T8*0.5</f>
+        <v>175</v>
+      </c>
+      <c r="V8" t="s" s="5">
+        <v>54</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6">
+        <v>40</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7">
         <v>5</v>
       </c>
       <c r="F9" t="s" s="5">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s" s="5">
-        <v>55</v>
-      </c>
-      <c r="H9" s="6">
+        <v>57</v>
+      </c>
+      <c r="H9" s="7">
         <v>1</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="7">
         <v>1</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7"/>
       <c r="L9" t="s" s="5">
-        <v>56</v>
-      </c>
-      <c r="M9" s="6">
+        <v>58</v>
+      </c>
+      <c r="M9" s="7">
         <v>60</v>
       </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" t="s" s="5">
-        <v>57</v>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="7">
+        <v>400</v>
+      </c>
+      <c r="U9" s="7">
+        <f>T9*0.5</f>
+        <v>200</v>
+      </c>
+      <c r="V9" t="s" s="5">
+        <v>59</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6">
+        <v>40</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7">
         <v>5</v>
       </c>
       <c r="F10" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s" s="5">
+        <v>62</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" t="s" s="5">
+        <v>63</v>
+      </c>
+      <c r="M10" s="7">
         <v>60</v>
       </c>
-      <c r="H10" s="6">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" t="s" s="5">
-        <v>61</v>
-      </c>
-      <c r="M10" s="6">
-        <v>60</v>
-      </c>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" t="s" s="5">
-        <v>62</v>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="7">
+        <v>450</v>
+      </c>
+      <c r="U10" s="7">
+        <f>T10*0.5</f>
+        <v>225</v>
+      </c>
+      <c r="V10" t="s" s="5">
+        <v>64</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6">
+        <v>40</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7">
         <v>5</v>
       </c>
       <c r="F11" t="s" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s" s="5">
-        <v>65</v>
-      </c>
-      <c r="H11" s="6">
+        <v>67</v>
+      </c>
+      <c r="H11" s="7">
         <v>1</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="7">
         <v>1</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" t="s" s="5">
-        <v>66</v>
-      </c>
-      <c r="M11" s="6">
+        <v>68</v>
+      </c>
+      <c r="M11" s="7">
         <v>60</v>
       </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" t="s" s="5">
-        <v>67</v>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="7">
+        <v>500</v>
+      </c>
+      <c r="U11" s="7">
+        <f>T11*0.5</f>
+        <v>250</v>
+      </c>
+      <c r="V11" t="s" s="5">
+        <v>69</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>50</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6">
+        <v>52</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7">
         <v>7</v>
       </c>
       <c r="F12" t="s" s="5">
-        <v>39</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="6">
+        <v>41</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="7">
         <v>-1</v>
       </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" t="s" s="5">
-        <v>70</v>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="7">
+        <v>550</v>
+      </c>
+      <c r="U12" s="7">
+        <f>T12*0.5</f>
+        <v>275</v>
+      </c>
+      <c r="V12" t="s" s="5">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
@@ -2617,26 +2567,26 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
+      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="8" customWidth="1"/>
-    <col min="2" max="2" width="8" style="8" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="8" customWidth="1"/>
-    <col min="4" max="4" width="2.375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="2.875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="5.25" style="8" customWidth="1"/>
-    <col min="7" max="7" width="5.625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="4.75" style="8" customWidth="1"/>
-    <col min="9" max="9" width="5.25" style="8" customWidth="1"/>
-    <col min="10" max="10" width="5.75" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.88281" style="8" customWidth="1"/>
-    <col min="12" max="12" width="6.25" style="8" customWidth="1"/>
-    <col min="13" max="13" width="6.375" style="8" customWidth="1"/>
-    <col min="14" max="14" width="31.2812" style="8" customWidth="1"/>
-    <col min="15" max="256" width="9" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.3516" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.6719" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.3516" style="9" customWidth="1"/>
+    <col min="4" max="4" width="3.17188" style="9" customWidth="1"/>
+    <col min="5" max="5" width="3.85156" style="9" customWidth="1"/>
+    <col min="6" max="6" width="7" style="9" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="6.35156" style="9" customWidth="1"/>
+    <col min="9" max="9" width="7" style="9" customWidth="1"/>
+    <col min="10" max="10" width="7.67188" style="9" customWidth="1"/>
+    <col min="11" max="11" width="11.8672" style="9" customWidth="1"/>
+    <col min="12" max="12" width="8.35156" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="9" customWidth="1"/>
+    <col min="14" max="14" width="41.6875" style="9" customWidth="1"/>
+    <col min="15" max="256" width="12" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -2656,19 +2606,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K1" t="s" s="2">
         <v>6</v>
@@ -2680,161 +2630,161 @@
         <v>11</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s" s="4">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>78</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7"/>
       <c r="K3" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="L3" s="6">
+        <v>28</v>
+      </c>
+      <c r="L3" s="7">
         <v>10</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="8"/>
       <c r="N3" t="s" s="5">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>82</v>
-      </c>
-      <c r="D4" s="5">
+        <v>84</v>
+      </c>
+      <c r="D4" s="6">
         <v>10</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
       <c r="N4" t="s" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>86</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
+        <v>88</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
         <v>10</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
       <c r="N5" t="s" s="5">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>88</v>
       </c>
-      <c r="B6" t="s" s="5">
-        <v>89</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>86</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6">
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
         <v>1</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
       <c r="N6" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>

</xml_diff>

<commit_message>
fixed #276 TournRPG-276 物理ブースター
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -344,11 +344,24 @@
             <rFont val="ヒラギノ角ゴ ProN W3"/>
           </rPr>
           <t>syun:
-耐性・ブースト上昇率(%)</t>
+attrのブースト上昇率(%)</t>
         </r>
       </text>
     </comment>
     <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+attrの耐性率(%)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -366,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>id</t>
   </si>
@@ -600,6 +613,12 @@
   </si>
   <si>
     <t>win_mp</t>
+  </si>
+  <si>
+    <t>boost</t>
+  </si>
+  <si>
+    <t>regist</t>
   </si>
   <si>
     <t>SKILL501</t>
@@ -2564,7 +2583,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2585,8 +2604,9 @@
     <col min="11" max="11" width="11.8672" style="9" customWidth="1"/>
     <col min="12" max="12" width="8.35156" style="9" customWidth="1"/>
     <col min="13" max="13" width="8.5" style="9" customWidth="1"/>
-    <col min="14" max="14" width="41.6875" style="9" customWidth="1"/>
-    <col min="15" max="256" width="12" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.5" style="9" customWidth="1"/>
+    <col min="15" max="15" width="41.6875" style="9" customWidth="1"/>
+    <col min="16" max="256" width="12" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -2624,12 +2644,15 @@
         <v>6</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="M1" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="N1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="O1" t="s" s="2">
         <v>21</v>
       </c>
     </row>
@@ -2670,22 +2693,23 @@
       <c r="L2" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="M2" t="s" s="4">
+      <c r="M2" s="4"/>
+      <c r="N2" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="N2" t="s" s="4">
+      <c r="O2" t="s" s="4">
         <v>23</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
@@ -2701,19 +2725,20 @@
         <v>10</v>
       </c>
       <c r="M3" s="8"/>
-      <c r="N3" t="s" s="5">
-        <v>81</v>
+      <c r="N3" s="8"/>
+      <c r="O3" t="s" s="5">
+        <v>83</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="6">
         <v>10</v>
@@ -2727,19 +2752,20 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
-      <c r="N4" t="s" s="5">
-        <v>85</v>
+      <c r="N4" s="8"/>
+      <c r="O4" t="s" s="5">
+        <v>87</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
@@ -2753,19 +2779,20 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" t="s" s="5">
-        <v>89</v>
+      <c r="N5" s="8"/>
+      <c r="O5" t="s" s="5">
+        <v>91</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>90</v>
-      </c>
-      <c r="B6" t="s" s="5">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>88</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
@@ -2779,8 +2806,9 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="N6" t="s" s="5">
-        <v>92</v>
+      <c r="N6" s="8"/>
+      <c r="O6" t="s" s="5">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #298 TournRPG-298 物理耐性
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
   <si>
     <t>id</t>
   </si>
@@ -664,6 +664,15 @@
   </si>
   <si>
     <t>死亡しても一度だけ復活</t>
+  </si>
+  <si>
+    <t>SKILL505</t>
+  </si>
+  <si>
+    <t>物理耐性</t>
+  </si>
+  <si>
+    <t>物理攻撃のダメージ減少</t>
   </si>
 </sst>
 </file>
@@ -2583,7 +2592,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2811,6 +2820,35 @@
         <v>94</v>
       </c>
     </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" t="s" s="3">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s" s="5">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="7"/>
+      <c r="K7" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="7">
+        <v>10</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" t="s" s="5">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
fixed #299 TournRPG-299 HP上昇
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -279,7 +279,7 @@
             <rFont val="ヒラギノ角ゴ ProN W3"/>
           </rPr>
           <t>syun:
-HP上昇率(%)</t>
+HP上昇値</t>
         </r>
       </text>
     </comment>
@@ -292,7 +292,33 @@
             <rFont val="ヒラギノ角ゴ ProN W3"/>
           </rPr>
           <t>syun:
-MP上昇率(%)</t>
+MP上昇値</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+ターン終了時にHP回復(%)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+ターン終了時にMP回復(%)</t>
         </r>
       </text>
     </comment>
@@ -332,6 +358,19 @@
           </rPr>
           <t>syun:
 戦闘勝利時にMP回復(%)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+ブースト・耐性の属性</t>
         </r>
       </text>
     </comment>
@@ -642,7 +681,7 @@
     <t>AUTO_STUP</t>
   </si>
   <si>
-    <t>最大HPが10%上昇</t>
+    <t>最大HPが10上昇</t>
   </si>
   <si>
     <t>SKILL503</t>

</xml_diff>

<commit_message>
fixed #301 TournRPG-301 バトル終了時にHP自動回復
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -721,6 +721,24 @@
   </si>
   <si>
     <t>ターン終了時にTPが5回復</t>
+  </si>
+  <si>
+    <t>SKILL507</t>
+  </si>
+  <si>
+    <t>天の加護</t>
+  </si>
+  <si>
+    <t>戦闘終了後にHPが15回復</t>
+  </si>
+  <si>
+    <t>SKILL508</t>
+  </si>
+  <si>
+    <t>ソウルヒール</t>
+  </si>
+  <si>
+    <t>戦闘終了後にMPが10回復</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2658,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2924,6 +2942,60 @@
         <v>100</v>
       </c>
     </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" t="s" s="3">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s" s="5">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>90</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7">
+        <v>15</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
+      <c r="O9" t="s" s="5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" t="s" s="3">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s" s="5">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>90</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="7">
+        <v>10</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+      <c r="O10" t="s" s="5">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
fixed #295 TournRPG-295 スキルコスト低下
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -413,12 +413,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+HPスキルコスト減少値</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+スキルコストMP減少値</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -660,6 +686,12 @@
     <t>regist</t>
   </si>
   <si>
+    <t>save_hp</t>
+  </si>
+  <si>
+    <t>save_mp</t>
+  </si>
+  <si>
     <t>SKILL501</t>
   </si>
   <si>
@@ -720,7 +752,7 @@
     <t>精神統一</t>
   </si>
   <si>
-    <t>ターン終了時にTPが5回復</t>
+    <t>ターン終了時にTPが1回復</t>
   </si>
   <si>
     <t>SKILL507</t>
@@ -738,7 +770,25 @@
     <t>ソウルヒール</t>
   </si>
   <si>
-    <t>戦闘終了後にMPが10回復</t>
+    <t>戦闘終了後にTPが10回復</t>
+  </si>
+  <si>
+    <t>SKILL509</t>
+  </si>
+  <si>
+    <t>武道の心得</t>
+  </si>
+  <si>
+    <t>スキルの消費HPが1減少</t>
+  </si>
+  <si>
+    <t>SKILL510</t>
+  </si>
+  <si>
+    <t>術理</t>
+  </si>
+  <si>
+    <t>スキルの消費TPが1減少</t>
   </si>
 </sst>
 </file>
@@ -2658,7 +2708,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2680,8 +2730,10 @@
     <col min="12" max="12" width="8.35156" style="9" customWidth="1"/>
     <col min="13" max="13" width="8.5" style="9" customWidth="1"/>
     <col min="14" max="14" width="8.5" style="9" customWidth="1"/>
-    <col min="15" max="15" width="41.6875" style="9" customWidth="1"/>
-    <col min="16" max="256" width="12" style="9" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="9" customWidth="1"/>
+    <col min="16" max="16" width="8.85156" style="9" customWidth="1"/>
+    <col min="17" max="17" width="41.6875" style="9" customWidth="1"/>
+    <col min="18" max="256" width="12" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -2728,6 +2780,12 @@
         <v>11</v>
       </c>
       <c r="O1" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P1" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="Q1" t="s" s="2">
         <v>21</v>
       </c>
     </row>
@@ -2768,23 +2826,31 @@
       <c r="L2" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" t="s" s="4">
+        <v>22</v>
+      </c>
       <c r="N2" t="s" s="4">
         <v>23</v>
       </c>
       <c r="O2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s" s="4">
         <v>23</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
@@ -2801,19 +2867,21 @@
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
-      <c r="O3" t="s" s="5">
-        <v>83</v>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" t="s" s="5">
+        <v>85</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D4" s="6">
         <v>10</v>
@@ -2828,19 +2896,21 @@
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="O4" t="s" s="5">
-        <v>87</v>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" t="s" s="5">
+        <v>89</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
@@ -2855,19 +2925,21 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="O5" t="s" s="5">
-        <v>91</v>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" t="s" s="5">
+        <v>93</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>92</v>
-      </c>
-      <c r="B6" t="s" s="5">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>90</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
@@ -2882,19 +2954,21 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" t="s" s="5">
-        <v>94</v>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" t="s" s="5">
+        <v>96</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="7"/>
@@ -2911,25 +2985,27 @@
         <v>10</v>
       </c>
       <c r="N7" s="8"/>
-      <c r="O7" t="s" s="5">
-        <v>97</v>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" t="s" s="5">
+        <v>99</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
@@ -2938,19 +3014,21 @@
       <c r="L8" s="8"/>
       <c r="M8" s="7"/>
       <c r="N8" s="8"/>
-      <c r="O8" t="s" s="5">
-        <v>100</v>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" t="s" s="5">
+        <v>102</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7"/>
@@ -2965,19 +3043,21 @@
       <c r="L9" s="8"/>
       <c r="M9" s="7"/>
       <c r="N9" s="8"/>
-      <c r="O9" t="s" s="5">
-        <v>103</v>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" t="s" s="5">
+        <v>105</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
@@ -2992,8 +3072,68 @@
       <c r="L10" s="8"/>
       <c r="M10" s="7"/>
       <c r="N10" s="8"/>
-      <c r="O10" t="s" s="5">
-        <v>106</v>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" t="s" s="5">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" t="s" s="3">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s" s="5">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>92</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="7">
+        <v>1</v>
+      </c>
+      <c r="P11" s="7"/>
+      <c r="Q11" t="s" s="5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" t="s" s="3">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s" s="5">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>92</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s" s="5">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #306 TournRPG-306 力上昇
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -305,7 +305,7 @@
             <rFont val="ヒラギノ角ゴ ProN W3"/>
           </rPr>
           <t>syun:
-ターン終了時にHP回復(%)</t>
+力上昇値</t>
         </r>
       </text>
     </comment>
@@ -318,7 +318,7 @@
             <rFont val="ヒラギノ角ゴ ProN W3"/>
           </rPr>
           <t>syun:
-ターン終了時にMP回復(%)</t>
+体力上昇値</t>
         </r>
       </text>
     </comment>
@@ -331,11 +331,50 @@
             <rFont val="ヒラギノ角ゴ ProN W3"/>
           </rPr>
           <t>syun:
+素早さ上昇値</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+ターン終了時にHP回復(%)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
+ターン終了時にMP回復(%)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="ヒラギノ角ゴ ProN W3"/>
+          </rPr>
+          <t>syun:
 HP0で一度だけ復活</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -348,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -361,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -374,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -387,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -444,7 +483,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="130">
   <si>
     <t>id</t>
   </si>
@@ -665,6 +704,15 @@
     <t>敵全体の攻撃力を下げる</t>
   </si>
   <si>
+    <t>vit</t>
+  </si>
+  <si>
+    <t>agi</t>
+  </si>
+  <si>
+    <t>mag</t>
+  </si>
+  <si>
     <t>rec_hp</t>
   </si>
   <si>
@@ -789,6 +837,42 @@
   </si>
   <si>
     <t>スキルの消費TPが1減少</t>
+  </si>
+  <si>
+    <t>SKILL511</t>
+  </si>
+  <si>
+    <t>力+2</t>
+  </si>
+  <si>
+    <t>力が1上昇</t>
+  </si>
+  <si>
+    <t>SKILL512</t>
+  </si>
+  <si>
+    <t>体力+3</t>
+  </si>
+  <si>
+    <t>体力が3上昇</t>
+  </si>
+  <si>
+    <t>SKILL513</t>
+  </si>
+  <si>
+    <t>素早さ+1</t>
+  </si>
+  <si>
+    <t>素早さが1上昇</t>
+  </si>
+  <si>
+    <t>SKILL514</t>
+  </si>
+  <si>
+    <t>魔力+2</t>
+  </si>
+  <si>
+    <t>魔力が2上昇</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2792,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2721,19 +2805,23 @@
     <col min="3" max="3" width="11.3516" style="9" customWidth="1"/>
     <col min="4" max="4" width="3.17188" style="9" customWidth="1"/>
     <col min="5" max="5" width="3.85156" style="9" customWidth="1"/>
-    <col min="6" max="6" width="7" style="9" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="9" customWidth="1"/>
-    <col min="8" max="8" width="6.35156" style="9" customWidth="1"/>
-    <col min="9" max="9" width="7" style="9" customWidth="1"/>
-    <col min="10" max="10" width="7.67188" style="9" customWidth="1"/>
-    <col min="11" max="11" width="11.8672" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.35156" style="9" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="9" customWidth="1"/>
-    <col min="14" max="14" width="8.5" style="9" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="9" customWidth="1"/>
-    <col min="16" max="16" width="8.85156" style="9" customWidth="1"/>
-    <col min="17" max="17" width="41.6875" style="9" customWidth="1"/>
-    <col min="18" max="256" width="12" style="9" customWidth="1"/>
+    <col min="6" max="6" width="3.5" style="9" customWidth="1"/>
+    <col min="7" max="7" width="3.17188" style="9" customWidth="1"/>
+    <col min="8" max="8" width="3.5" style="9" customWidth="1"/>
+    <col min="9" max="9" width="4.85156" style="9" customWidth="1"/>
+    <col min="10" max="10" width="7" style="9" customWidth="1"/>
+    <col min="11" max="11" width="7.5" style="9" customWidth="1"/>
+    <col min="12" max="12" width="6.35156" style="9" customWidth="1"/>
+    <col min="13" max="13" width="7" style="9" customWidth="1"/>
+    <col min="14" max="14" width="7.67188" style="9" customWidth="1"/>
+    <col min="15" max="15" width="11.8672" style="9" customWidth="1"/>
+    <col min="16" max="16" width="8.35156" style="9" customWidth="1"/>
+    <col min="17" max="17" width="8.5" style="9" customWidth="1"/>
+    <col min="18" max="18" width="8.5" style="9" customWidth="1"/>
+    <col min="19" max="19" width="8.5" style="9" customWidth="1"/>
+    <col min="20" max="20" width="8.85156" style="9" customWidth="1"/>
+    <col min="21" max="21" width="41.6875" style="9" customWidth="1"/>
+    <col min="22" max="256" width="12" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -2753,22 +2841,22 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="H1" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="I1" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="J1" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="K1" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="K1" t="s" s="2">
-        <v>6</v>
       </c>
       <c r="L1" t="s" s="2">
         <v>78</v>
@@ -2777,15 +2865,27 @@
         <v>79</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="P1" t="s" s="2">
         <v>81</v>
       </c>
       <c r="Q1" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="R1" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="T1" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="U1" t="s" s="2">
         <v>21</v>
       </c>
     </row>
@@ -2821,7 +2921,7 @@
         <v>22</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s" s="4">
         <v>22</v>
@@ -2830,58 +2930,74 @@
         <v>22</v>
       </c>
       <c r="N2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s" s="4">
         <v>23</v>
-      </c>
-      <c r="O2" t="s" s="4">
-        <v>22</v>
       </c>
       <c r="P2" t="s" s="4">
         <v>22</v>
       </c>
       <c r="Q2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="R2" t="s" s="4">
+        <v>23</v>
+      </c>
+      <c r="S2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="T2" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="U2" t="s" s="4">
         <v>23</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="3">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" t="s" s="5">
+      <c r="K3" s="7"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="7"/>
+      <c r="O3" t="s" s="5">
         <v>28</v>
       </c>
-      <c r="L3" s="7">
+      <c r="P3" s="7">
         <v>10</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" t="s" s="5">
-        <v>85</v>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" t="s" s="5">
+        <v>88</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D4" s="6">
         <v>10</v>
@@ -2889,251 +3005,419 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="N4" s="7"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
-      <c r="Q4" t="s" s="5">
-        <v>89</v>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" t="s" s="5">
+        <v>92</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7">
         <v>10</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="N5" s="7"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
-      <c r="Q5" t="s" s="5">
-        <v>93</v>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" t="s" s="5">
+        <v>96</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s" s="5">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>95</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>92</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="7">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
         <v>1</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="N6" s="7"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
-      <c r="Q6" t="s" s="5">
-        <v>96</v>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" t="s" s="5">
+        <v>99</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s" s="5">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" t="s" s="5">
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7"/>
+      <c r="O7" t="s" s="5">
         <v>28</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="7">
+      <c r="P7" s="8"/>
+      <c r="Q7" s="7">
         <v>10</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" t="s" s="5">
-        <v>99</v>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" t="s" s="5">
+        <v>102</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="7">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7">
         <v>1</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="5"/>
       <c r="P8" s="8"/>
-      <c r="Q8" t="s" s="5">
-        <v>102</v>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" t="s" s="5">
+        <v>105</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="7">
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7">
         <v>15</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="5"/>
       <c r="P9" s="8"/>
-      <c r="Q9" t="s" s="5">
-        <v>105</v>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" t="s" s="5">
+        <v>108</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="7">
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7">
         <v>10</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="O10" s="5"/>
       <c r="P10" s="8"/>
-      <c r="Q10" t="s" s="5">
-        <v>108</v>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" t="s" s="5">
+        <v>111</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="7">
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="7">
         <v>1</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" t="s" s="5">
-        <v>111</v>
+      <c r="T11" s="7"/>
+      <c r="U11" t="s" s="5">
+        <v>114</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="7">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="7">
         <v>1</v>
       </c>
-      <c r="Q12" t="s" s="5">
-        <v>114</v>
+      <c r="U12" t="s" s="5">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" t="s" s="3">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s" s="5">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
+        <v>2</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="7"/>
+      <c r="U13" t="s" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" t="s" s="3">
+        <v>121</v>
+      </c>
+      <c r="B14" t="s" s="5">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="7"/>
+      <c r="U14" t="s" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="A15" t="s" s="3">
+        <v>124</v>
+      </c>
+      <c r="B15" t="s" s="5">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="7"/>
+      <c r="U15" t="s" s="5">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s" s="5">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>91</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7">
+        <v>2</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="7"/>
+      <c r="U16" t="s" s="5">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #333 TournRPG-333 敵の作成
</commit_message>
<xml_diff>
--- a/docs/skill.xlsx
+++ b/docs/skill.xlsx
@@ -572,7 +572,10 @@
     <t>AT_PHY</t>
   </si>
   <si>
-    <t>敵1体に強力な攻撃をする</t>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>敵1体にかみつく。一定確率で毒</t>
   </si>
   <si>
     <t>SKILL002</t>
@@ -614,9 +617,6 @@
     <t>AT_POISON</t>
   </si>
   <si>
-    <t>poison</t>
-  </si>
-  <si>
     <t>敵全体に一定確率で毒</t>
   </si>
   <si>
@@ -659,7 +659,7 @@
     <t>AT_SLEEP</t>
   </si>
   <si>
-    <t>sleep</t>
+    <t>Sleep</t>
   </si>
   <si>
     <t>敵全体を一定確率で眠らせる</t>
@@ -674,7 +674,7 @@
     <t>AT_BLIND</t>
   </si>
   <si>
-    <t>blind</t>
+    <t>Blind</t>
   </si>
   <si>
     <t>相手を暗闇状態にする</t>
@@ -689,7 +689,7 @@
     <t>AT_CLOSE</t>
   </si>
   <si>
-    <t>close</t>
+    <t>Close</t>
   </si>
   <si>
     <t>相手のスキルを封印する</t>
@@ -2156,7 +2156,7 @@
     <col min="9" max="9" width="6.35156" style="1" customWidth="1"/>
     <col min="10" max="10" width="6.35156" style="1" customWidth="1"/>
     <col min="11" max="11" width="6.35156" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.35156" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.35156" style="1" customWidth="1"/>
     <col min="15" max="15" width="3.85156" style="1" customWidth="1"/>
@@ -2338,9 +2338,15 @@
       <c r="K3" s="7">
         <v>130</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="L3" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="M3" s="7">
+        <v>60</v>
+      </c>
+      <c r="N3" s="7">
+        <v>25</v>
+      </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -2354,15 +2360,15 @@
         <v>50</v>
       </c>
       <c r="V3" t="s" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s" s="5">
         <v>26</v>
@@ -2405,18 +2411,18 @@
         <v>75</v>
       </c>
       <c r="V4" t="s" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7">
@@ -2426,7 +2432,7 @@
         <v>27</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="7">
         <v>1</v>
@@ -2456,28 +2462,28 @@
         <v>100</v>
       </c>
       <c r="V5" t="s" s="5">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7">
         <v>3</v>
       </c>
       <c r="F6" t="s" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
@@ -2488,7 +2494,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" t="s" s="5">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="M6" s="7">
         <v>60</v>
@@ -2606,14 +2612,14 @@
         <v>56</v>
       </c>
       <c r="C9" t="s" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7">
         <v>5</v>
       </c>
       <c r="F9" t="s" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s" s="5">
         <v>57</v>
@@ -2657,7 +2663,7 @@
         <v>61</v>
       </c>
       <c r="C10" t="s" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7">
@@ -2708,7 +2714,7 @@
         <v>66</v>
       </c>
       <c r="C11" t="s" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="7">
@@ -2766,7 +2772,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
@@ -2809,7 +2815,7 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" t="s" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s" s="5">
         <v>28</v>

</xml_diff>